<commit_message>
Fixed output error on ED#
</commit_message>
<xml_diff>
--- a/TaskgraphsEdgeDetect/AlveoGenericSpecialized.xlsx
+++ b/TaskgraphsEdgeDetect/AlveoGenericSpecialized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Dev\Experiments\TaskgraphsEdgeDetect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3A1B1F-CED7-41AF-B14C-13C83829BB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EECD4C-E027-4E80-8B45-724837FDC6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27765" yWindow="2460" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specialized" sheetId="3" r:id="rId1"/>
@@ -369,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -388,9 +388,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -400,9 +397,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -417,13 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -436,35 +424,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -476,6 +437,48 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -772,237 +775,237 @@
     <col min="3" max="3" width="19" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="1"/>
-    <col min="6" max="6" width="27" style="39" customWidth="1"/>
+    <col min="6" max="6" width="27" style="28" customWidth="1"/>
     <col min="7" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="30" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="17">
         <v>27097</v>
       </c>
-      <c r="C2" s="40">
+      <c r="C2" s="35">
         <f>AVERAGE(B2:B6) / 1000</f>
         <v>27.248000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="41"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="1">
         <v>26809</v>
       </c>
-      <c r="C3" s="40"/>
+      <c r="C3" s="35"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="1">
         <v>27958</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="35"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
+      <c r="A5" s="34"/>
       <c r="B5" s="1">
         <v>26719</v>
       </c>
-      <c r="C5" s="40"/>
+      <c r="C5" s="35"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="6">
         <v>27657</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="35"/>
     </row>
     <row r="7" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7" s="17">
         <v>393408</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="35">
         <f>AVERAGE(B7:B11) / 1000</f>
         <v>393.73579999999998</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="1">
         <v>393693</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="35"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="1">
         <v>393577</v>
       </c>
-      <c r="C9" s="40"/>
+      <c r="C9" s="35"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="1">
         <v>393681</v>
       </c>
-      <c r="C10" s="40"/>
+      <c r="C10" s="35"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="6">
         <v>394320</v>
       </c>
-      <c r="C11" s="40"/>
+      <c r="C11" s="35"/>
     </row>
     <row r="12" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="17">
         <v>154045</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="35">
         <f>AVERAGE(B12:B16) / 1000</f>
         <v>153.73740000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="1">
         <v>153470</v>
       </c>
-      <c r="C13" s="40"/>
+      <c r="C13" s="35"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="1">
         <v>154048</v>
       </c>
-      <c r="C14" s="40"/>
+      <c r="C14" s="35"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="1">
         <v>153539</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="35"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="6">
         <v>153585</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="35"/>
     </row>
     <row r="17" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="17">
         <v>38734</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="35">
         <f>AVERAGE(B17:B21) / 1000</f>
         <v>38.290800000000004</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="1">
         <v>38106</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="F18" s="42"/>
+      <c r="C18" s="35"/>
+      <c r="F18" s="29"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="1">
         <v>38425</v>
       </c>
-      <c r="C19" s="40"/>
+      <c r="C19" s="35"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="1">
         <v>38395</v>
       </c>
-      <c r="C20" s="40"/>
+      <c r="C20" s="35"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="6">
         <v>37794</v>
       </c>
-      <c r="C21" s="40"/>
+      <c r="C21" s="35"/>
     </row>
     <row r="22" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="17">
         <v>155680</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="35">
         <f>AVERAGE(B22:B26) / 1000</f>
         <v>154.821</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="1">
         <v>154584</v>
       </c>
-      <c r="C23" s="40"/>
+      <c r="C23" s="35"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="1">
         <v>154733</v>
       </c>
-      <c r="C24" s="40"/>
+      <c r="C24" s="35"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="41"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="1">
         <v>154570</v>
       </c>
-      <c r="C25" s="40"/>
+      <c r="C25" s="35"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="6">
         <v>154538</v>
       </c>
-      <c r="C26" s="40"/>
+      <c r="C26" s="35"/>
     </row>
     <row r="27" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="40" t="e">
+      <c r="B27" s="17"/>
+      <c r="C27" s="35" t="e">
         <f>AVERAGE(B27:B31) / 1000</f>
         <v>#DIV/0!</v>
       </c>
@@ -1012,45 +1015,45 @@
       <c r="E27" s="1">
         <v>2607452</v>
       </c>
-      <c r="F27" s="39">
+      <c r="F27" s="28">
         <f>E27/(D27*1000000) * 1000</f>
         <v>8.6915066666666654</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="41"/>
-      <c r="C28" s="40"/>
+      <c r="A28" s="34"/>
+      <c r="C28" s="35"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="41"/>
-      <c r="C29" s="40"/>
+      <c r="A29" s="34"/>
+      <c r="C29" s="35"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="C30" s="40"/>
+      <c r="A30" s="34"/>
+      <c r="C30" s="35"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="40"/>
+      <c r="C31" s="35"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="C27:C31"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="C2:C6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="C7:C11"/>
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="C12:C16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="C27:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1063,7 +1066,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R11" sqref="R11"/>
+      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,210 +1075,212 @@
     <col min="2" max="2" width="17.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="9" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19" style="2" customWidth="1"/>
+    <col min="6" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="35" t="s">
+      <c r="D1" s="38"/>
+      <c r="E1" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="41"/>
+    </row>
+    <row r="2" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="43"/>
+      <c r="F2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="G2" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="H2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="I2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="J2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="20">
+        <v>320</v>
+      </c>
+      <c r="D3" s="19">
+        <v>200</v>
+      </c>
+      <c r="E3" s="15" t="e">
+        <f>AVERAGE(F3:J3) / 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="16"/>
+    </row>
+    <row r="4" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="45"/>
+      <c r="B4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C4" s="14">
         <v>512</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D4" s="13">
         <v>512</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="17" t="e">
-        <f>AVERAGE(E3:I3) / 1000</f>
+      <c r="E4" s="10" t="e">
+        <f>AVERAGE(F4:J4) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="15">
-        <v>320</v>
-      </c>
-      <c r="D4" s="14">
-        <v>200</v>
-      </c>
-      <c r="E4" s="13"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="11" t="e">
-        <f>AVERAGE(E4:I4) / 1000</f>
+      <c r="F4" s="12"/>
+      <c r="J4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="45"/>
+      <c r="B5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="14">
+        <v>640</v>
+      </c>
+      <c r="D5" s="13">
+        <v>480</v>
+      </c>
+      <c r="E5" s="10" t="e">
+        <f>AVERAGE(F5:J5) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="15">
-        <v>640</v>
-      </c>
-      <c r="D5" s="14">
+      <c r="F5" s="12"/>
+      <c r="J5" s="11"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
+      <c r="B6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="14">
+        <v>800</v>
+      </c>
+      <c r="D6" s="13">
         <v>480</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="11" t="e">
-        <f>AVERAGE(E5:I5) / 1000</f>
+      <c r="E6" s="10" t="e">
+        <f>AVERAGE(F6:J6) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="15">
+      <c r="F6" s="12"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="14">
         <v>800</v>
       </c>
-      <c r="D6" s="14">
-        <v>480</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="11" t="e">
-        <f>AVERAGE(E6:I6) / 1000</f>
+      <c r="D7" s="13">
+        <v>600</v>
+      </c>
+      <c r="E7" s="10" t="e">
+        <f>AVERAGE(F7:J7) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="15">
-        <v>800</v>
-      </c>
-      <c r="D7" s="14">
-        <v>600</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="11" t="e">
-        <f>AVERAGE(E7:I7) / 1000</f>
+      <c r="F7" s="12"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
+      <c r="B8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1280</v>
+      </c>
+      <c r="D8" s="13">
+        <v>720</v>
+      </c>
+      <c r="E8" s="10" t="e">
+        <f>AVERAGE(F8:J8) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="15">
-        <v>1280</v>
-      </c>
-      <c r="D8" s="14">
-        <v>720</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="11" t="e">
-        <f>AVERAGE(E8:I8) / 1000</f>
+      <c r="F8" s="12"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1920</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1080</v>
+      </c>
+      <c r="E9" s="10" t="e">
+        <f>AVERAGE(F9:J9) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="15">
-        <v>1920</v>
-      </c>
-      <c r="D9" s="14">
-        <v>1080</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="11" t="e">
-        <f>AVERAGE(E9:I9) / 1000</f>
+      <c r="F9" s="12"/>
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="45"/>
+      <c r="B10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14">
+        <v>2560</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1440</v>
+      </c>
+      <c r="E10" s="10" t="e">
+        <f>AVERAGE(F10:J10) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="15">
-        <v>2560</v>
-      </c>
-      <c r="D10" s="14">
-        <v>1440</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="11" t="e">
-        <f>AVERAGE(E10:I10) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="46"/>
       <c r="B11" s="9" t="s">
         <v>0</v>
       </c>
@@ -1285,167 +1290,229 @@
       <c r="D11" s="8">
         <v>2160</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="4" t="e">
+        <f>AVERAGE(F11:J11) / 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="7"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="4" t="e">
-        <f>AVERAGE(E11:I11) / 1000</f>
+      <c r="I11" s="6"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="20">
+        <v>320</v>
+      </c>
+      <c r="D12" s="19">
+        <v>200</v>
+      </c>
+      <c r="E12" s="15">
+        <f>AVERAGE(F12:J12) / 1000</f>
+        <v>92.747600000000006</v>
+      </c>
+      <c r="F12" s="18">
+        <v>92927</v>
+      </c>
+      <c r="G12" s="17">
+        <v>92756</v>
+      </c>
+      <c r="H12" s="17">
+        <v>92691</v>
+      </c>
+      <c r="I12" s="17">
+        <v>92594</v>
+      </c>
+      <c r="J12" s="16">
+        <v>92770</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="45"/>
+      <c r="B13" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="14">
+        <v>512</v>
+      </c>
+      <c r="D13" s="13">
+        <v>512</v>
+      </c>
+      <c r="E13" s="10">
+        <f>AVERAGE(F13:J13) / 1000</f>
+        <v>443.58820000000003</v>
+      </c>
+      <c r="F13" s="12">
+        <v>443457</v>
+      </c>
+      <c r="G13" s="1">
+        <v>443784</v>
+      </c>
+      <c r="H13" s="1">
+        <v>443452</v>
+      </c>
+      <c r="I13" s="1">
+        <v>443613</v>
+      </c>
+      <c r="J13" s="11">
+        <v>443635</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="45"/>
+      <c r="B14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="14">
+        <v>640</v>
+      </c>
+      <c r="D14" s="13">
+        <v>480</v>
+      </c>
+      <c r="E14" s="10">
+        <f>AVERAGE(F14:J14) / 1000</f>
+        <v>456.90120000000002</v>
+      </c>
+      <c r="F14" s="12">
+        <v>456914</v>
+      </c>
+      <c r="G14" s="1">
+        <v>456924</v>
+      </c>
+      <c r="H14" s="1">
+        <v>456981</v>
+      </c>
+      <c r="I14" s="1">
+        <v>456627</v>
+      </c>
+      <c r="J14" s="11">
+        <v>457060</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="45"/>
+      <c r="B15" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="14">
+        <v>800</v>
+      </c>
+      <c r="D15" s="13">
+        <v>480</v>
+      </c>
+      <c r="E15" s="10">
+        <f>AVERAGE(F15:J15) / 1000</f>
+        <v>513.65559999999994</v>
+      </c>
+      <c r="F15" s="12">
+        <v>513598</v>
+      </c>
+      <c r="G15" s="1">
+        <v>513677</v>
+      </c>
+      <c r="H15" s="1">
+        <v>513994</v>
+      </c>
+      <c r="I15" s="1">
+        <v>513463</v>
+      </c>
+      <c r="J15" s="11">
+        <v>513546</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="45"/>
+      <c r="B16" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="14">
+        <v>800</v>
+      </c>
+      <c r="D16" s="13">
+        <v>600</v>
+      </c>
+      <c r="E16" s="10">
+        <f>AVERAGE(F16:J16) / 1000</f>
+        <v>642.45980000000009</v>
+      </c>
+      <c r="F16" s="12">
+        <v>642555</v>
+      </c>
+      <c r="G16" s="1">
+        <v>642500</v>
+      </c>
+      <c r="H16" s="1">
+        <v>642525</v>
+      </c>
+      <c r="I16" s="1">
+        <v>642509</v>
+      </c>
+      <c r="J16" s="11">
+        <v>642210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
+      <c r="B17" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1280</v>
+      </c>
+      <c r="D17" s="13">
+        <v>720</v>
+      </c>
+      <c r="E17" s="10" t="e">
+        <f>AVERAGE(F17:J17) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="22">
-        <v>512</v>
-      </c>
-      <c r="D12" s="21">
-        <v>512</v>
-      </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="17" t="e">
-        <f>AVERAGE(E12:I12) / 1000</f>
+      <c r="F17" s="12"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="45"/>
+      <c r="B18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1920</v>
+      </c>
+      <c r="D18" s="13">
+        <v>1080</v>
+      </c>
+      <c r="E18" s="10" t="e">
+        <f>AVERAGE(F18:J18) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="15">
-        <v>320</v>
-      </c>
-      <c r="D13" s="14">
-        <v>200</v>
-      </c>
-      <c r="E13" s="13"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="11" t="e">
-        <f>AVERAGE(E13:I13) / 1000</f>
+      <c r="F18" s="12"/>
+      <c r="J18" s="11"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="45"/>
+      <c r="B19" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="14">
+        <v>2560</v>
+      </c>
+      <c r="D19" s="13">
+        <v>1440</v>
+      </c>
+      <c r="E19" s="10" t="e">
+        <f>AVERAGE(F19:J19) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="15">
-        <v>640</v>
-      </c>
-      <c r="D14" s="14">
-        <v>480</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="11" t="e">
-        <f>AVERAGE(E14:I14) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-      <c r="B15" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="15">
-        <v>800</v>
-      </c>
-      <c r="D15" s="14">
-        <v>480</v>
-      </c>
-      <c r="E15" s="13"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="11" t="e">
-        <f>AVERAGE(E15:I15) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="15">
-        <v>800</v>
-      </c>
-      <c r="D16" s="14">
-        <v>600</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="11" t="e">
-        <f>AVERAGE(E16:I16) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="15">
-        <v>1280</v>
-      </c>
-      <c r="D17" s="14">
-        <v>720</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="11" t="e">
-        <f>AVERAGE(E17:I17) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="15">
-        <v>1920</v>
-      </c>
-      <c r="D18" s="14">
-        <v>1080</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="11" t="e">
-        <f>AVERAGE(E18:I18) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="15">
-        <v>2560</v>
-      </c>
-      <c r="D19" s="14">
-        <v>1440</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="11" t="e">
-        <f>AVERAGE(E19:I19) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F19" s="12"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
+      <c r="A20" s="46"/>
       <c r="B20" s="9" t="s">
         <v>0</v>
       </c>
@@ -1455,167 +1522,229 @@
       <c r="D20" s="8">
         <v>2160</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="6"/>
+      <c r="E20" s="4" t="e">
+        <f>AVERAGE(F20:J20) / 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F20" s="7"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="4" t="e">
-        <f>AVERAGE(E20:I20) / 1000</f>
+      <c r="I20" s="6"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="20">
+        <v>320</v>
+      </c>
+      <c r="D21" s="19">
+        <v>200</v>
+      </c>
+      <c r="E21" s="15">
+        <f>AVERAGE(F21:J21) / 1000</f>
+        <v>85.691999999999993</v>
+      </c>
+      <c r="F21" s="18">
+        <v>85671</v>
+      </c>
+      <c r="G21" s="17">
+        <v>85652</v>
+      </c>
+      <c r="H21" s="17">
+        <v>85674</v>
+      </c>
+      <c r="I21" s="17">
+        <v>85712</v>
+      </c>
+      <c r="J21" s="16">
+        <v>85751</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="45"/>
+      <c r="B22" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="14">
+        <v>512</v>
+      </c>
+      <c r="D22" s="13">
+        <v>512</v>
+      </c>
+      <c r="E22" s="10">
+        <f>AVERAGE(F22:J22) / 1000</f>
+        <v>385.49420000000003</v>
+      </c>
+      <c r="F22" s="12">
+        <v>385400</v>
+      </c>
+      <c r="G22" s="1">
+        <v>385561</v>
+      </c>
+      <c r="H22" s="1">
+        <v>385541</v>
+      </c>
+      <c r="I22" s="1">
+        <v>385395</v>
+      </c>
+      <c r="J22" s="11">
+        <v>385574</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="45"/>
+      <c r="B23" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="14">
+        <v>640</v>
+      </c>
+      <c r="D23" s="13">
+        <v>480</v>
+      </c>
+      <c r="E23" s="10">
+        <f>AVERAGE(F23:J23) / 1000</f>
+        <v>411.46300000000002</v>
+      </c>
+      <c r="F23" s="12">
+        <v>411400</v>
+      </c>
+      <c r="G23" s="1">
+        <v>411664</v>
+      </c>
+      <c r="H23" s="1">
+        <v>411382</v>
+      </c>
+      <c r="I23" s="1">
+        <v>411545</v>
+      </c>
+      <c r="J23" s="11">
+        <v>411324</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="45"/>
+      <c r="B24" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="14">
+        <v>800</v>
+      </c>
+      <c r="D24" s="13">
+        <v>480</v>
+      </c>
+      <c r="E24" s="10">
+        <f>AVERAGE(F24:J24) / 1000</f>
+        <v>511.97640000000001</v>
+      </c>
+      <c r="F24" s="12">
+        <v>511970</v>
+      </c>
+      <c r="G24" s="1">
+        <v>512152</v>
+      </c>
+      <c r="H24" s="1">
+        <v>511899</v>
+      </c>
+      <c r="I24" s="1">
+        <v>512011</v>
+      </c>
+      <c r="J24" s="11">
+        <v>511850</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="45"/>
+      <c r="B25" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="14">
+        <v>800</v>
+      </c>
+      <c r="D25" s="13">
+        <v>600</v>
+      </c>
+      <c r="E25" s="10">
+        <f>AVERAGE(F25:J25) / 1000</f>
+        <v>640.01760000000002</v>
+      </c>
+      <c r="F25" s="12">
+        <v>640028</v>
+      </c>
+      <c r="G25" s="1">
+        <v>640131</v>
+      </c>
+      <c r="H25" s="1">
+        <v>639989</v>
+      </c>
+      <c r="I25" s="1">
+        <v>640021</v>
+      </c>
+      <c r="J25" s="11">
+        <v>639919</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="45"/>
+      <c r="B26" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="14">
+        <v>1280</v>
+      </c>
+      <c r="D26" s="13">
+        <v>720</v>
+      </c>
+      <c r="E26" s="10" t="e">
+        <f>AVERAGE(F26:J26) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="22">
-        <v>512</v>
-      </c>
-      <c r="D21" s="21">
-        <v>512</v>
-      </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="17" t="e">
-        <f>AVERAGE(E21:I21) / 1000</f>
+      <c r="F26" s="12"/>
+      <c r="J26" s="11"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="45"/>
+      <c r="B27" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="14">
+        <v>1920</v>
+      </c>
+      <c r="D27" s="13">
+        <v>1080</v>
+      </c>
+      <c r="E27" s="10" t="e">
+        <f>AVERAGE(F27:J27) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="15">
-        <v>320</v>
-      </c>
-      <c r="D22" s="14">
-        <v>200</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="11" t="e">
-        <f>AVERAGE(E22:I22) / 1000</f>
+      <c r="F27" s="12"/>
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="45"/>
+      <c r="B28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="14">
+        <v>2560</v>
+      </c>
+      <c r="D28" s="13">
+        <v>1440</v>
+      </c>
+      <c r="E28" s="10" t="e">
+        <f>AVERAGE(F28:J28) / 1000</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="15">
-        <v>640</v>
-      </c>
-      <c r="D23" s="14">
-        <v>480</v>
-      </c>
-      <c r="E23" s="13"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="11" t="e">
-        <f>AVERAGE(E23:I23) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="15">
-        <v>800</v>
-      </c>
-      <c r="D24" s="14">
-        <v>480</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="11" t="e">
-        <f>AVERAGE(E24:I24) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="15">
-        <v>800</v>
-      </c>
-      <c r="D25" s="14">
-        <v>600</v>
-      </c>
-      <c r="E25" s="13"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="11" t="e">
-        <f>AVERAGE(E25:I25) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="15">
-        <v>1280</v>
-      </c>
-      <c r="D26" s="14">
-        <v>720</v>
-      </c>
-      <c r="E26" s="13"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="11" t="e">
-        <f>AVERAGE(E26:I26) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="15">
-        <v>1920</v>
-      </c>
-      <c r="D27" s="14">
-        <v>1080</v>
-      </c>
-      <c r="E27" s="13"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="11" t="e">
-        <f>AVERAGE(E27:I27) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="15">
-        <v>2560</v>
-      </c>
-      <c r="D28" s="14">
-        <v>1440</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="11" t="e">
-        <f>AVERAGE(E28:I28) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="F28" s="12"/>
+      <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
+      <c r="A29" s="46"/>
       <c r="B29" s="9" t="s">
         <v>0</v>
       </c>
@@ -1625,21 +1754,21 @@
       <c r="D29" s="8">
         <v>2160</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="6"/>
+      <c r="E29" s="4" t="e">
+        <f>AVERAGE(F29:J29) / 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F29" s="7"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="4" t="e">
-        <f>AVERAGE(E29:I29) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="I29" s="6"/>
+      <c r="J29" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="A21:A29"/>
     <mergeCell ref="A12:A20"/>
     <mergeCell ref="A3:A11"/>

</xml_diff>

<commit_message>
Fixed segfault on ED
</commit_message>
<xml_diff>
--- a/TaskgraphsEdgeDetect/AlveoGenericSpecialized.xlsx
+++ b/TaskgraphsEdgeDetect/AlveoGenericSpecialized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Dev\Experiments\TaskgraphsEdgeDetect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EECD4C-E027-4E80-8B45-724837FDC6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324F5951-191D-42AC-AD22-B423241A18E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27765" yWindow="2460" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specialized" sheetId="3" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
-  <si>
-    <t>4K</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
   <si>
     <t>QHD</t>
   </si>
@@ -140,6 +137,19 @@
   </si>
   <si>
     <t>ExecTimes (us)</t>
+  </si>
+  <si>
+    <t>CPU Baseline
+AMD Ryzen Threadripper 3960X
+2.2GHz</t>
+  </si>
+  <si>
+    <t>CPU Baseline
+ARM Cortex-A57
+xxGhz</t>
+  </si>
+  <si>
+    <t>UHD</t>
   </si>
 </sst>
 </file>
@@ -369,7 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -479,6 +489,37 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -781,27 +822,27 @@
   <sheetData>
     <row r="1" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>21</v>
-      </c>
       <c r="D1" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="17">
         <v>27097</v>
@@ -841,7 +882,7 @@
     </row>
     <row r="7" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="17">
         <v>393408</v>
@@ -881,7 +922,7 @@
     </row>
     <row r="12" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="17">
         <v>154045</v>
@@ -921,7 +962,7 @@
     </row>
     <row r="17" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="17">
         <v>38734</v>
@@ -962,7 +1003,7 @@
     </row>
     <row r="22" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="17">
         <v>155680</v>
@@ -1002,7 +1043,7 @@
     </row>
     <row r="27" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="17"/>
       <c r="C27" s="35" t="e">
@@ -1062,16 +1103,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA35BC13-CFEA-4C5A-AA73-E4228B9F7178}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J33" sqref="J33"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
@@ -1082,16 +1123,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="38"/>
       <c r="E1" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="39" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>22</v>
       </c>
       <c r="G1" s="40"/>
       <c r="H1" s="40"/>
@@ -1100,40 +1141,40 @@
     </row>
     <row r="2" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="43"/>
       <c r="F2" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="20">
         <v>320</v>
@@ -1141,20 +1182,30 @@
       <c r="D3" s="19">
         <v>200</v>
       </c>
-      <c r="E3" s="15" t="e">
+      <c r="E3" s="15">
         <f>AVERAGE(F3:J3) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="16"/>
+        <v>10.192200000000001</v>
+      </c>
+      <c r="F3" s="49">
+        <v>10517</v>
+      </c>
+      <c r="G3" s="50">
+        <v>9681</v>
+      </c>
+      <c r="H3" s="50">
+        <v>10510</v>
+      </c>
+      <c r="I3" s="50">
+        <v>10516</v>
+      </c>
+      <c r="J3" s="51">
+        <v>9737</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="14">
         <v>512</v>
@@ -1162,17 +1213,30 @@
       <c r="D4" s="13">
         <v>512</v>
       </c>
-      <c r="E4" s="10" t="e">
+      <c r="E4" s="10">
         <f>AVERAGE(F4:J4) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="J4" s="11"/>
+        <v>25.382400000000001</v>
+      </c>
+      <c r="F4" s="52">
+        <v>25899</v>
+      </c>
+      <c r="G4" s="53">
+        <v>27069</v>
+      </c>
+      <c r="H4" s="53">
+        <v>27804</v>
+      </c>
+      <c r="I4" s="53">
+        <v>24715</v>
+      </c>
+      <c r="J4" s="54">
+        <v>21425</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="45"/>
       <c r="B5" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="14">
         <v>640</v>
@@ -1180,17 +1244,30 @@
       <c r="D5" s="13">
         <v>480</v>
       </c>
-      <c r="E5" s="10" t="e">
+      <c r="E5" s="10">
         <f>AVERAGE(F5:J5) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="J5" s="11"/>
+        <v>28.834</v>
+      </c>
+      <c r="F5" s="52">
+        <v>28915</v>
+      </c>
+      <c r="G5" s="53">
+        <v>30554</v>
+      </c>
+      <c r="H5" s="53">
+        <v>33053</v>
+      </c>
+      <c r="I5" s="53">
+        <v>25779</v>
+      </c>
+      <c r="J5" s="54">
+        <v>25869</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="45"/>
       <c r="B6" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="14">
         <v>800</v>
@@ -1198,17 +1275,30 @@
       <c r="D6" s="13">
         <v>480</v>
       </c>
-      <c r="E6" s="10" t="e">
+      <c r="E6" s="10">
         <f>AVERAGE(F6:J6) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="J6" s="11"/>
+        <v>33.4024</v>
+      </c>
+      <c r="F6" s="52">
+        <v>37653</v>
+      </c>
+      <c r="G6" s="53">
+        <v>32176</v>
+      </c>
+      <c r="H6" s="53">
+        <v>34704</v>
+      </c>
+      <c r="I6" s="53">
+        <v>31124</v>
+      </c>
+      <c r="J6" s="54">
+        <v>31355</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="45"/>
       <c r="B7" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="14">
         <v>800</v>
@@ -1216,17 +1306,30 @@
       <c r="D7" s="13">
         <v>600</v>
       </c>
-      <c r="E7" s="10" t="e">
+      <c r="E7" s="10">
         <f>AVERAGE(F7:J7) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="J7" s="11"/>
+        <v>45.034800000000004</v>
+      </c>
+      <c r="F7" s="52">
+        <v>43599</v>
+      </c>
+      <c r="G7" s="53">
+        <v>46654</v>
+      </c>
+      <c r="H7" s="53">
+        <v>47631</v>
+      </c>
+      <c r="I7" s="53">
+        <v>39945</v>
+      </c>
+      <c r="J7" s="54">
+        <v>47345</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="45"/>
       <c r="B8" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="14">
         <v>1280</v>
@@ -1234,17 +1337,30 @@
       <c r="D8" s="13">
         <v>720</v>
       </c>
-      <c r="E8" s="10" t="e">
+      <c r="E8" s="10">
         <f>AVERAGE(F8:J8) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="J8" s="11"/>
+        <v>81.890199999999993</v>
+      </c>
+      <c r="F8" s="52">
+        <v>82209</v>
+      </c>
+      <c r="G8" s="53">
+        <v>86472</v>
+      </c>
+      <c r="H8" s="53">
+        <v>79362</v>
+      </c>
+      <c r="I8" s="53">
+        <v>79429</v>
+      </c>
+      <c r="J8" s="54">
+        <v>81979</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="45"/>
       <c r="B9" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="14">
         <v>1920</v>
@@ -1252,17 +1368,30 @@
       <c r="D9" s="13">
         <v>1080</v>
       </c>
-      <c r="E9" s="10" t="e">
+      <c r="E9" s="10">
         <f>AVERAGE(F9:J9) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" s="12"/>
-      <c r="J9" s="11"/>
+        <v>186.0342</v>
+      </c>
+      <c r="F9" s="52">
+        <v>183965</v>
+      </c>
+      <c r="G9" s="53">
+        <v>181566</v>
+      </c>
+      <c r="H9" s="53">
+        <v>190148</v>
+      </c>
+      <c r="I9" s="53">
+        <v>186589</v>
+      </c>
+      <c r="J9" s="54">
+        <v>187903</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="45"/>
       <c r="B10" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="14">
         <v>2560</v>
@@ -1270,19 +1399,30 @@
       <c r="D10" s="13">
         <v>1440</v>
       </c>
-      <c r="E10" s="10" t="e">
+      <c r="E10" s="10">
         <f>AVERAGE(F10:J10) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="J10" s="11"/>
+        <v>313.57759999999996</v>
+      </c>
+      <c r="F10" s="52">
+        <v>317046</v>
+      </c>
+      <c r="G10" s="55">
+        <v>313201</v>
+      </c>
+      <c r="H10" s="55">
+        <v>316924</v>
+      </c>
+      <c r="I10" s="53">
+        <v>310436</v>
+      </c>
+      <c r="J10" s="54">
+        <v>310281</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
       <c r="B11" s="9" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C11" s="9">
         <v>3840</v>
@@ -1290,254 +1430,142 @@
       <c r="D11" s="8">
         <v>2160</v>
       </c>
-      <c r="E11" s="4" t="e">
+      <c r="E11" s="4">
         <f>AVERAGE(F11:J11) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>682.19319999999993</v>
+      </c>
+      <c r="F11" s="56">
+        <v>692792</v>
+      </c>
+      <c r="G11" s="57">
+        <v>674234</v>
+      </c>
+      <c r="H11" s="57">
+        <v>669037</v>
+      </c>
+      <c r="I11" s="57">
+        <v>701962</v>
+      </c>
+      <c r="J11" s="58">
+        <v>672941</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="20">
-        <v>320</v>
-      </c>
-      <c r="D12" s="19">
-        <v>200</v>
-      </c>
-      <c r="E12" s="15">
-        <f>AVERAGE(F12:J12) / 1000</f>
-        <v>92.747600000000006</v>
-      </c>
-      <c r="F12" s="18">
-        <v>92927</v>
-      </c>
-      <c r="G12" s="17">
-        <v>92756</v>
-      </c>
-      <c r="H12" s="17">
-        <v>92691</v>
-      </c>
-      <c r="I12" s="17">
-        <v>92594</v>
-      </c>
-      <c r="J12" s="16">
-        <v>92770</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="45"/>
-      <c r="B13" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="14">
-        <v>512</v>
-      </c>
-      <c r="D13" s="13">
-        <v>512</v>
-      </c>
-      <c r="E13" s="10">
-        <f>AVERAGE(F13:J13) / 1000</f>
-        <v>443.58820000000003</v>
-      </c>
-      <c r="F13" s="12">
-        <v>443457</v>
-      </c>
-      <c r="G13" s="1">
-        <v>443784</v>
-      </c>
-      <c r="H13" s="1">
-        <v>443452</v>
-      </c>
-      <c r="I13" s="1">
-        <v>443613</v>
-      </c>
-      <c r="J13" s="11">
-        <v>443635</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="45"/>
-      <c r="B14" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="14">
-        <v>640</v>
-      </c>
-      <c r="D14" s="13">
-        <v>480</v>
-      </c>
-      <c r="E14" s="10">
-        <f>AVERAGE(F14:J14) / 1000</f>
-        <v>456.90120000000002</v>
-      </c>
-      <c r="F14" s="12">
-        <v>456914</v>
-      </c>
-      <c r="G14" s="1">
-        <v>456924</v>
-      </c>
-      <c r="H14" s="1">
-        <v>456981</v>
-      </c>
-      <c r="I14" s="1">
-        <v>456627</v>
-      </c>
-      <c r="J14" s="11">
-        <v>457060</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="45"/>
-      <c r="B15" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="14">
-        <v>800</v>
-      </c>
-      <c r="D15" s="13">
-        <v>480</v>
-      </c>
-      <c r="E15" s="10">
-        <f>AVERAGE(F15:J15) / 1000</f>
-        <v>513.65559999999994</v>
-      </c>
-      <c r="F15" s="12">
-        <v>513598</v>
-      </c>
-      <c r="G15" s="1">
-        <v>513677</v>
-      </c>
-      <c r="H15" s="1">
-        <v>513994</v>
-      </c>
-      <c r="I15" s="1">
-        <v>513463</v>
-      </c>
-      <c r="J15" s="11">
-        <v>513546</v>
-      </c>
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="45"/>
-      <c r="B16" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="14">
-        <v>800</v>
-      </c>
-      <c r="D16" s="13">
-        <v>600</v>
-      </c>
-      <c r="E16" s="10">
-        <f>AVERAGE(F16:J16) / 1000</f>
-        <v>642.45980000000009</v>
-      </c>
-      <c r="F16" s="12">
-        <v>642555</v>
-      </c>
-      <c r="G16" s="1">
-        <v>642500</v>
-      </c>
-      <c r="H16" s="1">
-        <v>642525</v>
-      </c>
-      <c r="I16" s="1">
-        <v>642509</v>
-      </c>
-      <c r="J16" s="11">
-        <v>642210</v>
-      </c>
+      <c r="B16" s="47"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="45"/>
-      <c r="B17" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="14">
-        <v>1280</v>
-      </c>
-      <c r="D17" s="13">
-        <v>720</v>
-      </c>
-      <c r="E17" s="10" t="e">
-        <f>AVERAGE(F17:J17) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="12"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="45"/>
-      <c r="B18" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="14">
-        <v>1920</v>
-      </c>
-      <c r="D18" s="13">
-        <v>1080</v>
-      </c>
-      <c r="E18" s="10" t="e">
-        <f>AVERAGE(F18:J18) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="12"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="45"/>
-      <c r="B19" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="14">
-        <v>2560</v>
-      </c>
-      <c r="D19" s="13">
-        <v>1440</v>
-      </c>
-      <c r="E19" s="10" t="e">
-        <f>AVERAGE(F19:J19) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="12"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="46"/>
-      <c r="B20" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="9">
-        <v>3840</v>
-      </c>
-      <c r="D20" s="8">
-        <v>2160</v>
-      </c>
-      <c r="E20" s="4" t="e">
-        <f>AVERAGE(F20:J20) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="11"/>
+    </row>
+    <row r="21" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="20">
         <v>320</v>
@@ -1547,28 +1575,28 @@
       </c>
       <c r="E21" s="15">
         <f>AVERAGE(F21:J21) / 1000</f>
-        <v>85.691999999999993</v>
+        <v>92.747600000000006</v>
       </c>
       <c r="F21" s="18">
-        <v>85671</v>
+        <v>92927</v>
       </c>
       <c r="G21" s="17">
-        <v>85652</v>
+        <v>92756</v>
       </c>
       <c r="H21" s="17">
-        <v>85674</v>
+        <v>92691</v>
       </c>
       <c r="I21" s="17">
-        <v>85712</v>
+        <v>92594</v>
       </c>
       <c r="J21" s="16">
-        <v>85751</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>92770</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="45"/>
       <c r="B22" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="14">
         <v>512</v>
@@ -1578,28 +1606,28 @@
       </c>
       <c r="E22" s="10">
         <f>AVERAGE(F22:J22) / 1000</f>
-        <v>385.49420000000003</v>
+        <v>443.58820000000003</v>
       </c>
       <c r="F22" s="12">
-        <v>385400</v>
+        <v>443457</v>
       </c>
       <c r="G22" s="1">
-        <v>385561</v>
+        <v>443784</v>
       </c>
       <c r="H22" s="1">
-        <v>385541</v>
+        <v>443452</v>
       </c>
       <c r="I22" s="1">
-        <v>385395</v>
+        <v>443613</v>
       </c>
       <c r="J22" s="11">
-        <v>385574</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>443635</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="45"/>
       <c r="B23" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="14">
         <v>640</v>
@@ -1609,28 +1637,28 @@
       </c>
       <c r="E23" s="10">
         <f>AVERAGE(F23:J23) / 1000</f>
-        <v>411.46300000000002</v>
+        <v>456.90120000000002</v>
       </c>
       <c r="F23" s="12">
-        <v>411400</v>
+        <v>456914</v>
       </c>
       <c r="G23" s="1">
-        <v>411664</v>
+        <v>456924</v>
       </c>
       <c r="H23" s="1">
-        <v>411382</v>
+        <v>456981</v>
       </c>
       <c r="I23" s="1">
-        <v>411545</v>
+        <v>456627</v>
       </c>
       <c r="J23" s="11">
-        <v>411324</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>457060</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="45"/>
       <c r="B24" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="14">
         <v>800</v>
@@ -1640,28 +1668,28 @@
       </c>
       <c r="E24" s="10">
         <f>AVERAGE(F24:J24) / 1000</f>
-        <v>511.97640000000001</v>
+        <v>513.65559999999994</v>
       </c>
       <c r="F24" s="12">
-        <v>511970</v>
+        <v>513598</v>
       </c>
       <c r="G24" s="1">
-        <v>512152</v>
+        <v>513677</v>
       </c>
       <c r="H24" s="1">
-        <v>511899</v>
+        <v>513994</v>
       </c>
       <c r="I24" s="1">
-        <v>512011</v>
+        <v>513463</v>
       </c>
       <c r="J24" s="11">
-        <v>511850</v>
+        <v>513546</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="45"/>
       <c r="B25" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" s="14">
         <v>800</v>
@@ -1671,28 +1699,28 @@
       </c>
       <c r="E25" s="10">
         <f>AVERAGE(F25:J25) / 1000</f>
-        <v>640.01760000000002</v>
+        <v>642.45980000000009</v>
       </c>
       <c r="F25" s="12">
-        <v>640028</v>
+        <v>642555</v>
       </c>
       <c r="G25" s="1">
-        <v>640131</v>
+        <v>642500</v>
       </c>
       <c r="H25" s="1">
-        <v>639989</v>
+        <v>642525</v>
       </c>
       <c r="I25" s="1">
-        <v>640021</v>
+        <v>642509</v>
       </c>
       <c r="J25" s="11">
-        <v>639919</v>
+        <v>642210</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="45"/>
       <c r="B26" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" s="14">
         <v>1280</v>
@@ -1700,17 +1728,30 @@
       <c r="D26" s="13">
         <v>720</v>
       </c>
-      <c r="E26" s="10" t="e">
+      <c r="E26" s="10">
         <f>AVERAGE(F26:J26) / 1000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F26" s="12"/>
-      <c r="J26" s="11"/>
+        <v>1382.5319999999999</v>
+      </c>
+      <c r="F26" s="12">
+        <v>1382416</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1382296</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1382503</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1383013</v>
+      </c>
+      <c r="J26" s="11">
+        <v>1382432</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="45"/>
       <c r="B27" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="14">
         <v>1920</v>
@@ -1728,7 +1769,7 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="45"/>
       <c r="B28" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" s="14">
         <v>2560</v>
@@ -1746,7 +1787,7 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="46"/>
       <c r="B29" s="9" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C29" s="9">
         <v>3840</v>
@@ -1764,14 +1805,260 @@
       <c r="I29" s="6"/>
       <c r="J29" s="5"/>
     </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="20">
+        <v>320</v>
+      </c>
+      <c r="D30" s="19">
+        <v>200</v>
+      </c>
+      <c r="E30" s="15">
+        <f>AVERAGE(F30:J30) / 1000</f>
+        <v>85.691999999999993</v>
+      </c>
+      <c r="F30" s="18">
+        <v>85671</v>
+      </c>
+      <c r="G30" s="17">
+        <v>85652</v>
+      </c>
+      <c r="H30" s="17">
+        <v>85674</v>
+      </c>
+      <c r="I30" s="17">
+        <v>85712</v>
+      </c>
+      <c r="J30" s="16">
+        <v>85751</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="45"/>
+      <c r="B31" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="14">
+        <v>512</v>
+      </c>
+      <c r="D31" s="13">
+        <v>512</v>
+      </c>
+      <c r="E31" s="10">
+        <f>AVERAGE(F31:J31) / 1000</f>
+        <v>385.49420000000003</v>
+      </c>
+      <c r="F31" s="12">
+        <v>385400</v>
+      </c>
+      <c r="G31" s="1">
+        <v>385561</v>
+      </c>
+      <c r="H31" s="1">
+        <v>385541</v>
+      </c>
+      <c r="I31" s="1">
+        <v>385395</v>
+      </c>
+      <c r="J31" s="11">
+        <v>385574</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="45"/>
+      <c r="B32" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="14">
+        <v>640</v>
+      </c>
+      <c r="D32" s="13">
+        <v>480</v>
+      </c>
+      <c r="E32" s="10">
+        <f>AVERAGE(F32:J32) / 1000</f>
+        <v>411.46300000000002</v>
+      </c>
+      <c r="F32" s="12">
+        <v>411400</v>
+      </c>
+      <c r="G32" s="1">
+        <v>411664</v>
+      </c>
+      <c r="H32" s="1">
+        <v>411382</v>
+      </c>
+      <c r="I32" s="1">
+        <v>411545</v>
+      </c>
+      <c r="J32" s="11">
+        <v>411324</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="45"/>
+      <c r="B33" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="14">
+        <v>800</v>
+      </c>
+      <c r="D33" s="13">
+        <v>480</v>
+      </c>
+      <c r="E33" s="10">
+        <f>AVERAGE(F33:J33) / 1000</f>
+        <v>511.97640000000001</v>
+      </c>
+      <c r="F33" s="12">
+        <v>511970</v>
+      </c>
+      <c r="G33" s="1">
+        <v>512152</v>
+      </c>
+      <c r="H33" s="1">
+        <v>511899</v>
+      </c>
+      <c r="I33" s="1">
+        <v>512011</v>
+      </c>
+      <c r="J33" s="11">
+        <v>511850</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="45"/>
+      <c r="B34" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="14">
+        <v>800</v>
+      </c>
+      <c r="D34" s="13">
+        <v>600</v>
+      </c>
+      <c r="E34" s="10">
+        <f>AVERAGE(F34:J34) / 1000</f>
+        <v>640.01760000000002</v>
+      </c>
+      <c r="F34" s="12">
+        <v>640028</v>
+      </c>
+      <c r="G34" s="1">
+        <v>640131</v>
+      </c>
+      <c r="H34" s="1">
+        <v>639989</v>
+      </c>
+      <c r="I34" s="1">
+        <v>640021</v>
+      </c>
+      <c r="J34" s="11">
+        <v>639919</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="45"/>
+      <c r="B35" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="14">
+        <v>1280</v>
+      </c>
+      <c r="D35" s="13">
+        <v>720</v>
+      </c>
+      <c r="E35" s="10">
+        <f>AVERAGE(F35:J35) / 1000</f>
+        <v>1294.9296000000002</v>
+      </c>
+      <c r="F35" s="12">
+        <v>1295159</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1295698</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1295257</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1294609</v>
+      </c>
+      <c r="J35" s="11">
+        <v>1293925</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="45"/>
+      <c r="B36" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="14">
+        <v>1920</v>
+      </c>
+      <c r="D36" s="13">
+        <v>1080</v>
+      </c>
+      <c r="E36" s="10" t="e">
+        <f>AVERAGE(F36:J36) / 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="J36" s="11"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="45"/>
+      <c r="B37" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="14">
+        <v>2560</v>
+      </c>
+      <c r="D37" s="13">
+        <v>1440</v>
+      </c>
+      <c r="E37" s="10" t="e">
+        <f>AVERAGE(F37:J37) / 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F37" s="12"/>
+      <c r="J37" s="11"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="46"/>
+      <c r="B38" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="9">
+        <v>3840</v>
+      </c>
+      <c r="D38" s="8">
+        <v>2160</v>
+      </c>
+      <c r="E38" s="4" t="e">
+        <f>AVERAGE(F38:J38) / 1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="E1:E2"/>
+    <mergeCell ref="A30:A38"/>
     <mergeCell ref="A21:A29"/>
+    <mergeCell ref="A3:A11"/>
     <mergeCell ref="A12:A20"/>
-    <mergeCell ref="A3:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
CPU data for Alveo
</commit_message>
<xml_diff>
--- a/TaskgraphsEdgeDetect/AlveoGenericSpecialized.xlsx
+++ b/TaskgraphsEdgeDetect/AlveoGenericSpecialized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Dev\Experiments\TaskgraphsEdgeDetect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324F5951-191D-42AC-AD22-B423241A18E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D2D962-300D-47D6-BFCB-FFED6565AC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specialized" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>QHD</t>
   </si>
@@ -139,17 +139,17 @@
     <t>ExecTimes (us)</t>
   </si>
   <si>
+    <t>UHD</t>
+  </si>
+  <si>
+    <t>CPU Baseline
+ARM Cortex-A57
+1479MHz (max)</t>
+  </si>
+  <si>
     <t>CPU Baseline
 AMD Ryzen Threadripper 3960X
-2.2GHz</t>
-  </si>
-  <si>
-    <t>CPU Baseline
-ARM Cortex-A57
-xxGhz</t>
-  </si>
-  <si>
-    <t>UHD</t>
+4568MHz (max)</t>
   </si>
 </sst>
 </file>
@@ -234,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -374,12 +374,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -520,6 +531,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1107,7 +1121,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1185,7 @@
     </row>
     <row r="3" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="20" t="s">
         <v>6</v>
@@ -1422,7 +1436,7 @@
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
       <c r="B11" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="9">
         <v>3840</v>
@@ -1454,111 +1468,282 @@
       <c r="A12" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="11"/>
+      <c r="B12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="20">
+        <v>320</v>
+      </c>
+      <c r="D12" s="19">
+        <v>200</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" ref="E12:E20" si="0">AVERAGE(F12:J12) / 1000</f>
+        <v>28.3752</v>
+      </c>
+      <c r="F12" s="12">
+        <v>30432</v>
+      </c>
+      <c r="G12" s="48">
+        <v>28281</v>
+      </c>
+      <c r="H12" s="48">
+        <v>27613</v>
+      </c>
+      <c r="I12" s="48">
+        <v>27674</v>
+      </c>
+      <c r="J12" s="11">
+        <v>27876</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="45"/>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="11"/>
+      <c r="B13" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="14">
+        <v>512</v>
+      </c>
+      <c r="D13" s="47">
+        <v>512</v>
+      </c>
+      <c r="E13" s="59">
+        <f t="shared" si="0"/>
+        <v>112.2342</v>
+      </c>
+      <c r="F13" s="48">
+        <v>114828</v>
+      </c>
+      <c r="G13" s="48">
+        <v>112229</v>
+      </c>
+      <c r="H13" s="48">
+        <v>111416</v>
+      </c>
+      <c r="I13" s="48">
+        <v>111210</v>
+      </c>
+      <c r="J13" s="11">
+        <v>111488</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="45"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="11"/>
+      <c r="B14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="14">
+        <v>640</v>
+      </c>
+      <c r="D14" s="47">
+        <v>480</v>
+      </c>
+      <c r="E14" s="59">
+        <f t="shared" si="0"/>
+        <v>130.96039999999999</v>
+      </c>
+      <c r="F14" s="48">
+        <v>132606</v>
+      </c>
+      <c r="G14" s="48">
+        <v>130504</v>
+      </c>
+      <c r="H14" s="48">
+        <v>130450</v>
+      </c>
+      <c r="I14" s="48">
+        <v>130530</v>
+      </c>
+      <c r="J14" s="11">
+        <v>130712</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="45"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="11"/>
+      <c r="B15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="14">
+        <v>800</v>
+      </c>
+      <c r="D15" s="47">
+        <v>480</v>
+      </c>
+      <c r="E15" s="59">
+        <f t="shared" si="0"/>
+        <v>164.20179999999999</v>
+      </c>
+      <c r="F15" s="48">
+        <v>165670</v>
+      </c>
+      <c r="G15" s="48">
+        <v>163847</v>
+      </c>
+      <c r="H15" s="48">
+        <v>163852</v>
+      </c>
+      <c r="I15" s="48">
+        <v>163699</v>
+      </c>
+      <c r="J15" s="11">
+        <v>163941</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="45"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="11"/>
+      <c r="B16" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="14">
+        <v>800</v>
+      </c>
+      <c r="D16" s="47">
+        <v>600</v>
+      </c>
+      <c r="E16" s="59">
+        <f t="shared" si="0"/>
+        <v>203.75620000000001</v>
+      </c>
+      <c r="F16" s="48">
+        <v>205320</v>
+      </c>
+      <c r="G16" s="48">
+        <v>204050</v>
+      </c>
+      <c r="H16" s="48">
+        <v>202553</v>
+      </c>
+      <c r="I16" s="48">
+        <v>202371</v>
+      </c>
+      <c r="J16" s="11">
+        <v>204487</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="45"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="11"/>
+      <c r="B17" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1280</v>
+      </c>
+      <c r="D17" s="47">
+        <v>720</v>
+      </c>
+      <c r="E17" s="59">
+        <f t="shared" si="0"/>
+        <v>397.93579999999997</v>
+      </c>
+      <c r="F17" s="48">
+        <v>400967</v>
+      </c>
+      <c r="G17" s="48">
+        <v>398775</v>
+      </c>
+      <c r="H17" s="48">
+        <v>398350</v>
+      </c>
+      <c r="I17" s="48">
+        <v>395735</v>
+      </c>
+      <c r="J17" s="11">
+        <v>395852</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="45"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="11"/>
+      <c r="B18" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="14">
+        <v>1920</v>
+      </c>
+      <c r="D18" s="47">
+        <v>1080</v>
+      </c>
+      <c r="E18" s="59">
+        <f t="shared" si="0"/>
+        <v>910.41759999999999</v>
+      </c>
+      <c r="F18" s="48">
+        <v>918508</v>
+      </c>
+      <c r="G18" s="48">
+        <v>918147</v>
+      </c>
+      <c r="H18" s="48">
+        <v>905967</v>
+      </c>
+      <c r="I18" s="48">
+        <v>904861</v>
+      </c>
+      <c r="J18" s="11">
+        <v>904605</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="45"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="11"/>
+      <c r="B19" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="14">
+        <v>2560</v>
+      </c>
+      <c r="D19" s="47">
+        <v>1440</v>
+      </c>
+      <c r="E19" s="59">
+        <f t="shared" si="0"/>
+        <v>1651.3044</v>
+      </c>
+      <c r="F19" s="48">
+        <v>1649938</v>
+      </c>
+      <c r="G19" s="48">
+        <v>1654203</v>
+      </c>
+      <c r="H19" s="48">
+        <v>1659457</v>
+      </c>
+      <c r="I19" s="48">
+        <v>1649401</v>
+      </c>
+      <c r="J19" s="11">
+        <v>1643523</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="46"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="11"/>
+      <c r="B20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="9">
+        <v>3840</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2160</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>3733.3557999999998</v>
+      </c>
+      <c r="F20" s="12">
+        <v>3714559</v>
+      </c>
+      <c r="G20" s="48">
+        <v>3736907</v>
+      </c>
+      <c r="H20" s="48">
+        <v>3732772</v>
+      </c>
+      <c r="I20" s="48">
+        <v>3741147</v>
+      </c>
+      <c r="J20" s="11">
+        <v>3741394</v>
+      </c>
     </row>
     <row r="21" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
@@ -1787,7 +1972,7 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="46"/>
       <c r="B29" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C29" s="9">
         <v>3840</v>
@@ -2032,7 +2217,7 @@
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="46"/>
       <c r="B38" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C38" s="9">
         <v>3840</v>

</xml_diff>

<commit_message>
Changes in ILP stuff
</commit_message>
<xml_diff>
--- a/TaskgraphsEdgeDetect/AlveoGenericSpecialized.xlsx
+++ b/TaskgraphsEdgeDetect/AlveoGenericSpecialized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Dev\Experiments\TaskgraphsEdgeDetect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D2D962-300D-47D6-BFCB-FFED6565AC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB437DE-8CC2-469A-9A77-5795EEDCFCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specialized" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>QHD</t>
   </si>
@@ -150,6 +150,18 @@
     <t>CPU Baseline
 AMD Ryzen Threadripper 3960X
 4568MHz (max)</t>
+  </si>
+  <si>
+    <t>V0</t>
+  </si>
+  <si>
+    <t>V0CE</t>
+  </si>
+  <si>
+    <t>CPU AMD</t>
+  </si>
+  <si>
+    <t>CPU ARM</t>
   </si>
 </sst>
 </file>
@@ -390,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -459,6 +471,39 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -497,43 +542,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -551,6 +559,1250 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Generic!$P$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V0CE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Generic!$Q$3:$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>HD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SVGA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WVGA</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VGA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DEFAULT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CGA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Generic!$Q$4:$V$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1294.9296000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>640.01760000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>511.97640000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>411.46300000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>385.49420000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85.691999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-424B-436F-9268-F528564D0B36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Generic!$P$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>V0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Generic!$Q$3:$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>HD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SVGA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WVGA</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VGA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DEFAULT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CGA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Generic!$Q$5:$V$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1382.5319999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>642.45980000000009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>513.65559999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>456.90120000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>443.58820000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>92.747600000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-424B-436F-9268-F528564D0B36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Generic!$P$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPU ARM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Generic!$Q$3:$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>HD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SVGA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WVGA</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VGA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DEFAULT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CGA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Generic!$Q$6:$V$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>397.93579999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>203.75620000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>164.20179999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130.96039999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>112.2342</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.3752</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-424B-436F-9268-F528564D0B36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Generic!$P$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPU AMD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Generic!$Q$3:$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>HD</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SVGA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WVGA</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VGA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DEFAULT</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>CGA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Generic!$Q$7:$V$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>81.890199999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45.034800000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.4024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.834</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.382400000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.192200000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-424B-436F-9268-F528564D0B36}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="111879903"/>
+        <c:axId val="111886559"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="111879903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Image Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="111886559"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="111886559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Execution Time (us)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="111879903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400" b="1"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98AE24BC-E5AC-F5EB-0F20-05D9C4CF5212}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -855,212 +2107,212 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="45" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="17">
         <v>27097</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="46">
         <f>AVERAGE(B2:B6) / 1000</f>
         <v>27.248000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="1">
         <v>26809</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="46"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="34"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="1">
         <v>27958</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="46"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="34"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="1">
         <v>26719</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="46"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="6">
         <v>27657</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="46"/>
     </row>
     <row r="7" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="45" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="17">
         <v>393408</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="46">
         <f>AVERAGE(B7:B11) / 1000</f>
         <v>393.73579999999998</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
+      <c r="A8" s="45"/>
       <c r="B8" s="1">
         <v>393693</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="46"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="1">
         <v>393577</v>
       </c>
-      <c r="C9" s="35"/>
+      <c r="C9" s="46"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="45"/>
       <c r="B10" s="1">
         <v>393681</v>
       </c>
-      <c r="C10" s="35"/>
+      <c r="C10" s="46"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="6">
         <v>394320</v>
       </c>
-      <c r="C11" s="35"/>
+      <c r="C11" s="46"/>
     </row>
     <row r="12" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="45" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="17">
         <v>154045</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="46">
         <f>AVERAGE(B12:B16) / 1000</f>
         <v>153.73740000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="A13" s="45"/>
       <c r="B13" s="1">
         <v>153470</v>
       </c>
-      <c r="C13" s="35"/>
+      <c r="C13" s="46"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="1">
         <v>154048</v>
       </c>
-      <c r="C14" s="35"/>
+      <c r="C14" s="46"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="45"/>
       <c r="B15" s="1">
         <v>153539</v>
       </c>
-      <c r="C15" s="35"/>
+      <c r="C15" s="46"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="45"/>
       <c r="B16" s="6">
         <v>153585</v>
       </c>
-      <c r="C16" s="35"/>
+      <c r="C16" s="46"/>
     </row>
     <row r="17" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="45" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="17">
         <v>38734</v>
       </c>
-      <c r="C17" s="35">
+      <c r="C17" s="46">
         <f>AVERAGE(B17:B21) / 1000</f>
         <v>38.290800000000004</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
+      <c r="A18" s="45"/>
       <c r="B18" s="1">
         <v>38106</v>
       </c>
-      <c r="C18" s="35"/>
+      <c r="C18" s="46"/>
       <c r="F18" s="29"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="1">
         <v>38425</v>
       </c>
-      <c r="C19" s="35"/>
+      <c r="C19" s="46"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="34"/>
+      <c r="A20" s="45"/>
       <c r="B20" s="1">
         <v>38395</v>
       </c>
-      <c r="C20" s="35"/>
+      <c r="C20" s="46"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
+      <c r="A21" s="45"/>
       <c r="B21" s="6">
         <v>37794</v>
       </c>
-      <c r="C21" s="35"/>
+      <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="45" t="s">
         <v>24</v>
       </c>
       <c r="B22" s="17">
         <v>155680</v>
       </c>
-      <c r="C22" s="35">
+      <c r="C22" s="46">
         <f>AVERAGE(B22:B26) / 1000</f>
         <v>154.821</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="34"/>
+      <c r="A23" s="45"/>
       <c r="B23" s="1">
         <v>154584</v>
       </c>
-      <c r="C23" s="35"/>
+      <c r="C23" s="46"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="34"/>
+      <c r="A24" s="45"/>
       <c r="B24" s="1">
         <v>154733</v>
       </c>
-      <c r="C24" s="35"/>
+      <c r="C24" s="46"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="34"/>
+      <c r="A25" s="45"/>
       <c r="B25" s="1">
         <v>154570</v>
       </c>
-      <c r="C25" s="35"/>
+      <c r="C25" s="46"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="34"/>
+      <c r="A26" s="45"/>
       <c r="B26" s="6">
         <v>154538</v>
       </c>
-      <c r="C26" s="35"/>
+      <c r="C26" s="46"/>
     </row>
     <row r="27" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="45" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="17"/>
-      <c r="C27" s="35" t="e">
+      <c r="C27" s="46" t="e">
         <f>AVERAGE(B27:B31) / 1000</f>
         <v>#DIV/0!</v>
       </c>
@@ -1076,21 +2328,21 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="C28" s="35"/>
+      <c r="A28" s="45"/>
+      <c r="C28" s="46"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="34"/>
-      <c r="C29" s="35"/>
+      <c r="A29" s="45"/>
+      <c r="C29" s="46"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="34"/>
-      <c r="C30" s="35"/>
+      <c r="A30" s="45"/>
+      <c r="C30" s="46"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="34"/>
+      <c r="A31" s="45"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="35"/>
+      <c r="C31" s="46"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
@@ -1117,11 +2369,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA35BC13-CFEA-4C5A-AA73-E4228B9F7178}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:A20"/>
+      <selection pane="bottomLeft" activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,28 +2384,30 @@
     <col min="4" max="4" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" style="2" customWidth="1"/>
     <col min="6" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.5703125" style="1"/>
+    <col min="11" max="15" width="8.5703125" style="1"/>
+    <col min="16" max="16" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="42" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="41"/>
-    </row>
-    <row r="2" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="52"/>
+    </row>
+    <row r="2" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>19</v>
       </c>
@@ -1166,7 +2420,7 @@
       <c r="D2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="43"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="24" t="s">
         <v>15</v>
       </c>
@@ -1183,8 +2437,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+    <row r="3" spans="1:22" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="55" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -1197,27 +2451,45 @@
         <v>200</v>
       </c>
       <c r="E3" s="15">
-        <f>AVERAGE(F3:J3) / 1000</f>
+        <f t="shared" ref="E3:E11" si="0">AVERAGE(F3:J3) / 1000</f>
         <v>10.192200000000001</v>
       </c>
-      <c r="F3" s="49">
+      <c r="F3" s="34">
         <v>10517</v>
       </c>
-      <c r="G3" s="50">
+      <c r="G3" s="35">
         <v>9681</v>
       </c>
-      <c r="H3" s="50">
+      <c r="H3" s="35">
         <v>10510</v>
       </c>
-      <c r="I3" s="50">
+      <c r="I3" s="35">
         <v>10516</v>
       </c>
-      <c r="J3" s="51">
+      <c r="J3" s="36">
         <v>9737</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
+      <c r="Q3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="56"/>
       <c r="B4" s="14" t="s">
         <v>7</v>
       </c>
@@ -1228,27 +2500,48 @@
         <v>512</v>
       </c>
       <c r="E4" s="10">
-        <f>AVERAGE(F4:J4) / 1000</f>
+        <f t="shared" si="0"/>
         <v>25.382400000000001</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="37">
         <v>25899</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="38">
         <v>27069</v>
       </c>
-      <c r="H4" s="53">
+      <c r="H4" s="38">
         <v>27804</v>
       </c>
-      <c r="I4" s="53">
+      <c r="I4" s="38">
         <v>24715</v>
       </c>
-      <c r="J4" s="54">
+      <c r="J4" s="39">
         <v>21425</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="45"/>
+      <c r="P4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1294.9296000000002</v>
+      </c>
+      <c r="R4" s="1">
+        <v>640.01760000000002</v>
+      </c>
+      <c r="S4" s="1">
+        <v>511.97640000000001</v>
+      </c>
+      <c r="T4" s="1">
+        <v>411.46300000000002</v>
+      </c>
+      <c r="U4" s="1">
+        <v>385.49420000000003</v>
+      </c>
+      <c r="V4" s="1">
+        <v>85.691999999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="56"/>
       <c r="B5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1259,27 +2552,48 @@
         <v>480</v>
       </c>
       <c r="E5" s="10">
-        <f>AVERAGE(F5:J5) / 1000</f>
+        <f t="shared" si="0"/>
         <v>28.834</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="37">
         <v>28915</v>
       </c>
-      <c r="G5" s="53">
+      <c r="G5" s="38">
         <v>30554</v>
       </c>
-      <c r="H5" s="53">
+      <c r="H5" s="38">
         <v>33053</v>
       </c>
-      <c r="I5" s="53">
+      <c r="I5" s="38">
         <v>25779</v>
       </c>
-      <c r="J5" s="54">
+      <c r="J5" s="39">
         <v>25869</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
+      <c r="P5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>1382.5319999999999</v>
+      </c>
+      <c r="R5" s="1">
+        <v>642.45980000000009</v>
+      </c>
+      <c r="S5" s="1">
+        <v>513.65559999999994</v>
+      </c>
+      <c r="T5" s="1">
+        <v>456.90120000000002</v>
+      </c>
+      <c r="U5" s="1">
+        <v>443.58820000000003</v>
+      </c>
+      <c r="V5" s="1">
+        <v>92.747600000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="56"/>
       <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
@@ -1290,27 +2604,48 @@
         <v>480</v>
       </c>
       <c r="E6" s="10">
-        <f>AVERAGE(F6:J6) / 1000</f>
+        <f t="shared" si="0"/>
         <v>33.4024</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="37">
         <v>37653</v>
       </c>
-      <c r="G6" s="53">
+      <c r="G6" s="38">
         <v>32176</v>
       </c>
-      <c r="H6" s="53">
+      <c r="H6" s="38">
         <v>34704</v>
       </c>
-      <c r="I6" s="53">
+      <c r="I6" s="38">
         <v>31124</v>
       </c>
-      <c r="J6" s="54">
+      <c r="J6" s="39">
         <v>31355</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
+      <c r="P6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>397.93579999999997</v>
+      </c>
+      <c r="R6" s="1">
+        <v>203.75620000000001</v>
+      </c>
+      <c r="S6" s="1">
+        <v>164.20179999999999</v>
+      </c>
+      <c r="T6" s="1">
+        <v>130.96039999999999</v>
+      </c>
+      <c r="U6" s="1">
+        <v>112.2342</v>
+      </c>
+      <c r="V6" s="1">
+        <v>28.3752</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="56"/>
       <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
@@ -1321,27 +2656,48 @@
         <v>600</v>
       </c>
       <c r="E7" s="10">
-        <f>AVERAGE(F7:J7) / 1000</f>
+        <f t="shared" si="0"/>
         <v>45.034800000000004</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="37">
         <v>43599</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="38">
         <v>46654</v>
       </c>
-      <c r="H7" s="53">
+      <c r="H7" s="38">
         <v>47631</v>
       </c>
-      <c r="I7" s="53">
+      <c r="I7" s="38">
         <v>39945</v>
       </c>
-      <c r="J7" s="54">
+      <c r="J7" s="39">
         <v>47345</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
+      <c r="P7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>81.890199999999993</v>
+      </c>
+      <c r="R7" s="1">
+        <v>45.034800000000004</v>
+      </c>
+      <c r="S7" s="1">
+        <v>33.4024</v>
+      </c>
+      <c r="T7" s="1">
+        <v>28.834</v>
+      </c>
+      <c r="U7" s="1">
+        <v>25.382400000000001</v>
+      </c>
+      <c r="V7" s="1">
+        <v>10.192200000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="56"/>
       <c r="B8" s="14" t="s">
         <v>2</v>
       </c>
@@ -1352,27 +2708,27 @@
         <v>720</v>
       </c>
       <c r="E8" s="10">
-        <f>AVERAGE(F8:J8) / 1000</f>
+        <f t="shared" si="0"/>
         <v>81.890199999999993</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="37">
         <v>82209</v>
       </c>
-      <c r="G8" s="53">
+      <c r="G8" s="38">
         <v>86472</v>
       </c>
-      <c r="H8" s="53">
+      <c r="H8" s="38">
         <v>79362</v>
       </c>
-      <c r="I8" s="53">
+      <c r="I8" s="38">
         <v>79429</v>
       </c>
-      <c r="J8" s="54">
+      <c r="J8" s="39">
         <v>81979</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" s="56"/>
       <c r="B9" s="14" t="s">
         <v>1</v>
       </c>
@@ -1383,27 +2739,27 @@
         <v>1080</v>
       </c>
       <c r="E9" s="10">
-        <f>AVERAGE(F9:J9) / 1000</f>
+        <f t="shared" si="0"/>
         <v>186.0342</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="37">
         <v>183965</v>
       </c>
-      <c r="G9" s="53">
+      <c r="G9" s="38">
         <v>181566</v>
       </c>
-      <c r="H9" s="53">
+      <c r="H9" s="38">
         <v>190148</v>
       </c>
-      <c r="I9" s="53">
+      <c r="I9" s="38">
         <v>186589</v>
       </c>
-      <c r="J9" s="54">
+      <c r="J9" s="39">
         <v>187903</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="56"/>
       <c r="B10" s="14" t="s">
         <v>0</v>
       </c>
@@ -1414,27 +2770,27 @@
         <v>1440</v>
       </c>
       <c r="E10" s="10">
-        <f>AVERAGE(F10:J10) / 1000</f>
+        <f t="shared" si="0"/>
         <v>313.57759999999996</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="37">
         <v>317046</v>
       </c>
-      <c r="G10" s="55">
+      <c r="G10" s="40">
         <v>313201</v>
       </c>
-      <c r="H10" s="55">
+      <c r="H10" s="40">
         <v>316924</v>
       </c>
-      <c r="I10" s="53">
+      <c r="I10" s="38">
         <v>310436</v>
       </c>
-      <c r="J10" s="54">
+      <c r="J10" s="39">
         <v>310281</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" s="57"/>
       <c r="B11" s="9" t="s">
         <v>32</v>
       </c>
@@ -1445,27 +2801,27 @@
         <v>2160</v>
       </c>
       <c r="E11" s="4">
-        <f>AVERAGE(F11:J11) / 1000</f>
+        <f t="shared" si="0"/>
         <v>682.19319999999993</v>
       </c>
-      <c r="F11" s="56">
+      <c r="F11" s="41">
         <v>692792</v>
       </c>
-      <c r="G11" s="57">
+      <c r="G11" s="42">
         <v>674234</v>
       </c>
-      <c r="H11" s="57">
+      <c r="H11" s="42">
         <v>669037</v>
       </c>
-      <c r="I11" s="57">
+      <c r="I11" s="42">
         <v>701962</v>
       </c>
-      <c r="J11" s="58">
+      <c r="J11" s="43">
         <v>672941</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="55" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -1478,143 +2834,143 @@
         <v>200</v>
       </c>
       <c r="E12" s="10">
-        <f t="shared" ref="E12:E20" si="0">AVERAGE(F12:J12) / 1000</f>
+        <f t="shared" ref="E12:E20" si="1">AVERAGE(F12:J12) / 1000</f>
         <v>28.3752</v>
       </c>
       <c r="F12" s="12">
         <v>30432</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="1">
         <v>28281</v>
       </c>
-      <c r="H12" s="48">
+      <c r="H12" s="1">
         <v>27613</v>
       </c>
-      <c r="I12" s="48">
+      <c r="I12" s="1">
         <v>27674</v>
       </c>
       <c r="J12" s="11">
         <v>27876</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="45"/>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="56"/>
       <c r="B13" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="14">
         <v>512</v>
       </c>
-      <c r="D13" s="47">
+      <c r="D13" s="14">
         <v>512</v>
       </c>
-      <c r="E13" s="59">
-        <f t="shared" si="0"/>
+      <c r="E13" s="44">
+        <f t="shared" si="1"/>
         <v>112.2342</v>
       </c>
-      <c r="F13" s="48">
+      <c r="F13" s="1">
         <v>114828</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="1">
         <v>112229</v>
       </c>
-      <c r="H13" s="48">
+      <c r="H13" s="1">
         <v>111416</v>
       </c>
-      <c r="I13" s="48">
+      <c r="I13" s="1">
         <v>111210</v>
       </c>
       <c r="J13" s="11">
         <v>111488</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" s="56"/>
       <c r="B14" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="14">
         <v>640</v>
       </c>
-      <c r="D14" s="47">
+      <c r="D14" s="14">
         <v>480</v>
       </c>
-      <c r="E14" s="59">
-        <f t="shared" si="0"/>
+      <c r="E14" s="44">
+        <f t="shared" si="1"/>
         <v>130.96039999999999</v>
       </c>
-      <c r="F14" s="48">
+      <c r="F14" s="1">
         <v>132606</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="1">
         <v>130504</v>
       </c>
-      <c r="H14" s="48">
+      <c r="H14" s="1">
         <v>130450</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="1">
         <v>130530</v>
       </c>
       <c r="J14" s="11">
         <v>130712</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" s="56"/>
       <c r="B15" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="14">
         <v>800</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="14">
         <v>480</v>
       </c>
-      <c r="E15" s="59">
-        <f t="shared" si="0"/>
+      <c r="E15" s="44">
+        <f t="shared" si="1"/>
         <v>164.20179999999999</v>
       </c>
-      <c r="F15" s="48">
+      <c r="F15" s="1">
         <v>165670</v>
       </c>
-      <c r="G15" s="48">
+      <c r="G15" s="1">
         <v>163847</v>
       </c>
-      <c r="H15" s="48">
+      <c r="H15" s="1">
         <v>163852</v>
       </c>
-      <c r="I15" s="48">
+      <c r="I15" s="1">
         <v>163699</v>
       </c>
       <c r="J15" s="11">
         <v>163941</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="56"/>
       <c r="B16" s="14" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="14">
         <v>800</v>
       </c>
-      <c r="D16" s="47">
+      <c r="D16" s="14">
         <v>600</v>
       </c>
-      <c r="E16" s="59">
-        <f t="shared" si="0"/>
+      <c r="E16" s="44">
+        <f t="shared" si="1"/>
         <v>203.75620000000001</v>
       </c>
-      <c r="F16" s="48">
+      <c r="F16" s="1">
         <v>205320</v>
       </c>
-      <c r="G16" s="48">
+      <c r="G16" s="1">
         <v>204050</v>
       </c>
-      <c r="H16" s="48">
+      <c r="H16" s="1">
         <v>202553</v>
       </c>
-      <c r="I16" s="48">
+      <c r="I16" s="1">
         <v>202371</v>
       </c>
       <c r="J16" s="11">
@@ -1622,30 +2978,30 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="45"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="14" t="s">
         <v>2</v>
       </c>
       <c r="C17" s="14">
         <v>1280</v>
       </c>
-      <c r="D17" s="47">
+      <c r="D17" s="14">
         <v>720</v>
       </c>
-      <c r="E17" s="59">
-        <f t="shared" si="0"/>
+      <c r="E17" s="44">
+        <f t="shared" si="1"/>
         <v>397.93579999999997</v>
       </c>
-      <c r="F17" s="48">
+      <c r="F17" s="1">
         <v>400967</v>
       </c>
-      <c r="G17" s="48">
+      <c r="G17" s="1">
         <v>398775</v>
       </c>
-      <c r="H17" s="48">
+      <c r="H17" s="1">
         <v>398350</v>
       </c>
-      <c r="I17" s="48">
+      <c r="I17" s="1">
         <v>395735</v>
       </c>
       <c r="J17" s="11">
@@ -1653,30 +3009,30 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="14">
         <v>1920</v>
       </c>
-      <c r="D18" s="47">
+      <c r="D18" s="14">
         <v>1080</v>
       </c>
-      <c r="E18" s="59">
-        <f t="shared" si="0"/>
+      <c r="E18" s="44">
+        <f t="shared" si="1"/>
         <v>910.41759999999999</v>
       </c>
-      <c r="F18" s="48">
+      <c r="F18" s="1">
         <v>918508</v>
       </c>
-      <c r="G18" s="48">
+      <c r="G18" s="1">
         <v>918147</v>
       </c>
-      <c r="H18" s="48">
+      <c r="H18" s="1">
         <v>905967</v>
       </c>
-      <c r="I18" s="48">
+      <c r="I18" s="1">
         <v>904861</v>
       </c>
       <c r="J18" s="11">
@@ -1684,30 +3040,30 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="14">
         <v>2560</v>
       </c>
-      <c r="D19" s="47">
+      <c r="D19" s="14">
         <v>1440</v>
       </c>
-      <c r="E19" s="59">
-        <f t="shared" si="0"/>
+      <c r="E19" s="44">
+        <f t="shared" si="1"/>
         <v>1651.3044</v>
       </c>
-      <c r="F19" s="48">
+      <c r="F19" s="1">
         <v>1649938</v>
       </c>
-      <c r="G19" s="48">
+      <c r="G19" s="1">
         <v>1654203</v>
       </c>
-      <c r="H19" s="48">
+      <c r="H19" s="1">
         <v>1659457</v>
       </c>
-      <c r="I19" s="48">
+      <c r="I19" s="1">
         <v>1649401</v>
       </c>
       <c r="J19" s="11">
@@ -1715,7 +3071,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
+      <c r="A20" s="57"/>
       <c r="B20" s="9" t="s">
         <v>32</v>
       </c>
@@ -1726,19 +3082,19 @@
         <v>2160</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3733.3557999999998</v>
       </c>
       <c r="F20" s="12">
         <v>3714559</v>
       </c>
-      <c r="G20" s="48">
+      <c r="G20" s="1">
         <v>3736907</v>
       </c>
-      <c r="H20" s="48">
+      <c r="H20" s="1">
         <v>3732772</v>
       </c>
-      <c r="I20" s="48">
+      <c r="I20" s="1">
         <v>3741147</v>
       </c>
       <c r="J20" s="11">
@@ -1746,7 +3102,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="55" t="s">
         <v>9</v>
       </c>
       <c r="B21" s="20" t="s">
@@ -1759,7 +3115,7 @@
         <v>200</v>
       </c>
       <c r="E21" s="15">
-        <f>AVERAGE(F21:J21) / 1000</f>
+        <f t="shared" ref="E21:E38" si="2">AVERAGE(F21:J21) / 1000</f>
         <v>92.747600000000006</v>
       </c>
       <c r="F21" s="18">
@@ -1779,7 +3135,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="56"/>
       <c r="B22" s="14" t="s">
         <v>7</v>
       </c>
@@ -1790,7 +3146,7 @@
         <v>512</v>
       </c>
       <c r="E22" s="10">
-        <f>AVERAGE(F22:J22) / 1000</f>
+        <f t="shared" si="2"/>
         <v>443.58820000000003</v>
       </c>
       <c r="F22" s="12">
@@ -1810,7 +3166,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45"/>
+      <c r="A23" s="56"/>
       <c r="B23" s="14" t="s">
         <v>5</v>
       </c>
@@ -1821,7 +3177,7 @@
         <v>480</v>
       </c>
       <c r="E23" s="10">
-        <f>AVERAGE(F23:J23) / 1000</f>
+        <f t="shared" si="2"/>
         <v>456.90120000000002</v>
       </c>
       <c r="F23" s="12">
@@ -1841,7 +3197,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="45"/>
+      <c r="A24" s="56"/>
       <c r="B24" s="14" t="s">
         <v>4</v>
       </c>
@@ -1852,7 +3208,7 @@
         <v>480</v>
       </c>
       <c r="E24" s="10">
-        <f>AVERAGE(F24:J24) / 1000</f>
+        <f t="shared" si="2"/>
         <v>513.65559999999994</v>
       </c>
       <c r="F24" s="12">
@@ -1872,7 +3228,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="45"/>
+      <c r="A25" s="56"/>
       <c r="B25" s="14" t="s">
         <v>3</v>
       </c>
@@ -1883,7 +3239,7 @@
         <v>600</v>
       </c>
       <c r="E25" s="10">
-        <f>AVERAGE(F25:J25) / 1000</f>
+        <f t="shared" si="2"/>
         <v>642.45980000000009</v>
       </c>
       <c r="F25" s="12">
@@ -1903,7 +3259,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
+      <c r="A26" s="56"/>
       <c r="B26" s="14" t="s">
         <v>2</v>
       </c>
@@ -1914,7 +3270,7 @@
         <v>720</v>
       </c>
       <c r="E26" s="10">
-        <f>AVERAGE(F26:J26) / 1000</f>
+        <f t="shared" si="2"/>
         <v>1382.5319999999999</v>
       </c>
       <c r="F26" s="12">
@@ -1934,7 +3290,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="45"/>
+      <c r="A27" s="56"/>
       <c r="B27" s="14" t="s">
         <v>1</v>
       </c>
@@ -1945,14 +3301,14 @@
         <v>1080</v>
       </c>
       <c r="E27" s="10" t="e">
-        <f>AVERAGE(F27:J27) / 1000</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F27" s="12"/>
       <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="45"/>
+      <c r="A28" s="56"/>
       <c r="B28" s="14" t="s">
         <v>0</v>
       </c>
@@ -1963,14 +3319,14 @@
         <v>1440</v>
       </c>
       <c r="E28" s="10" t="e">
-        <f>AVERAGE(F28:J28) / 1000</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F28" s="12"/>
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
+      <c r="A29" s="57"/>
       <c r="B29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1981,7 +3337,7 @@
         <v>2160</v>
       </c>
       <c r="E29" s="4" t="e">
-        <f>AVERAGE(F29:J29) / 1000</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F29" s="7"/>
@@ -1991,7 +3347,7 @@
       <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="55" t="s">
         <v>8</v>
       </c>
       <c r="B30" s="20" t="s">
@@ -2004,7 +3360,7 @@
         <v>200</v>
       </c>
       <c r="E30" s="15">
-        <f>AVERAGE(F30:J30) / 1000</f>
+        <f t="shared" si="2"/>
         <v>85.691999999999993</v>
       </c>
       <c r="F30" s="18">
@@ -2024,7 +3380,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="14" t="s">
         <v>7</v>
       </c>
@@ -2035,7 +3391,7 @@
         <v>512</v>
       </c>
       <c r="E31" s="10">
-        <f>AVERAGE(F31:J31) / 1000</f>
+        <f t="shared" si="2"/>
         <v>385.49420000000003</v>
       </c>
       <c r="F31" s="12">
@@ -2055,7 +3411,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="45"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="14" t="s">
         <v>5</v>
       </c>
@@ -2066,7 +3422,7 @@
         <v>480</v>
       </c>
       <c r="E32" s="10">
-        <f>AVERAGE(F32:J32) / 1000</f>
+        <f t="shared" si="2"/>
         <v>411.46300000000002</v>
       </c>
       <c r="F32" s="12">
@@ -2086,7 +3442,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="45"/>
+      <c r="A33" s="56"/>
       <c r="B33" s="14" t="s">
         <v>4</v>
       </c>
@@ -2097,7 +3453,7 @@
         <v>480</v>
       </c>
       <c r="E33" s="10">
-        <f>AVERAGE(F33:J33) / 1000</f>
+        <f t="shared" si="2"/>
         <v>511.97640000000001</v>
       </c>
       <c r="F33" s="12">
@@ -2117,7 +3473,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
+      <c r="A34" s="56"/>
       <c r="B34" s="14" t="s">
         <v>3</v>
       </c>
@@ -2128,7 +3484,7 @@
         <v>600</v>
       </c>
       <c r="E34" s="10">
-        <f>AVERAGE(F34:J34) / 1000</f>
+        <f t="shared" si="2"/>
         <v>640.01760000000002</v>
       </c>
       <c r="F34" s="12">
@@ -2148,7 +3504,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="45"/>
+      <c r="A35" s="56"/>
       <c r="B35" s="14" t="s">
         <v>2</v>
       </c>
@@ -2159,7 +3515,7 @@
         <v>720</v>
       </c>
       <c r="E35" s="10">
-        <f>AVERAGE(F35:J35) / 1000</f>
+        <f t="shared" si="2"/>
         <v>1294.9296000000002</v>
       </c>
       <c r="F35" s="12">
@@ -2179,7 +3535,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="45"/>
+      <c r="A36" s="56"/>
       <c r="B36" s="14" t="s">
         <v>1</v>
       </c>
@@ -2190,14 +3546,14 @@
         <v>1080</v>
       </c>
       <c r="E36" s="10" t="e">
-        <f>AVERAGE(F36:J36) / 1000</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F36" s="12"/>
       <c r="J36" s="11"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="45"/>
+      <c r="A37" s="56"/>
       <c r="B37" s="14" t="s">
         <v>0</v>
       </c>
@@ -2208,14 +3564,14 @@
         <v>1440</v>
       </c>
       <c r="E37" s="10" t="e">
-        <f>AVERAGE(F37:J37) / 1000</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F37" s="12"/>
       <c r="J37" s="11"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
+      <c r="A38" s="57"/>
       <c r="B38" s="9" t="s">
         <v>32</v>
       </c>
@@ -2226,7 +3582,7 @@
         <v>2160</v>
       </c>
       <c r="E38" s="4" t="e">
-        <f>AVERAGE(F38:J38) / 1000</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F38" s="7"/>
@@ -2247,5 +3603,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>